<commit_message>
combine all markdowns and tests
</commit_message>
<xml_diff>
--- a/data/test_meal_logs.xlsx
+++ b/data/test_meal_logs.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,29 +494,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2 parathas with curd</t>
+          <t>Had 3 idlis for breakfast</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-01-12T14:39:48.865712</t>
+          <t>2026-01-14T17:17:48.419079</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Evening Snack</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2x paratha, 1x curd</t>
+          <t>3x idli</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>350</v>
+        <v>117</v>
       </c>
       <c r="G2" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -532,29 +532,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Had 3 idlis for breakfast</t>
+          <t>Ate chicken biryani</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-12T14:39:48.858221</t>
+          <t>2026-01-14T17:17:48.412534</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Evening Snack</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3x idli</t>
+          <t>1x biryani</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>117</v>
+        <v>280</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -570,69 +570,31 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ate chicken biryani and raita</t>
+          <t>I had 2 rotis and dal</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2026-01-12T14:39:48.849181</t>
+          <t>2026-01-14T17:17:48.404366</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Evening Snack</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1x biryani, 1x raita</t>
+          <t>2x roti, 1x dal</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>347</v>
+        <v>246</v>
       </c>
       <c r="G4" t="n">
-        <v>15.5</v>
+        <v>13.8</v>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>testing</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>whatsapp:+1234567890</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>I had 2 rotis and dal</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2026-01-12T14:39:48.842094</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2x roti, 1x dal</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>246</v>
-      </c>
-      <c r="G5" t="n">
-        <v>13.8</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>testing</t>
         </is>

</xml_diff>

<commit_message>
bug fix for adding food
</commit_message>
<xml_diff>
--- a/data/test_meal_logs.xlsx
+++ b/data/test_meal_logs.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-01-15T16:03:58.872145</t>
+          <t>2026-01-15T16:19:14.711087</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-15T16:03:58.865210</t>
+          <t>2026-01-15T16:19:14.702643</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2026-01-15T16:03:58.860934</t>
+          <t>2026-01-15T16:19:14.698272</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>